<commit_message>
one strike in frist frame
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="6">
   <si>
     <t>X</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:W25"/>
+  <dimension ref="A2:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,95 +919,127 @@
         <v>0</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="V12" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="C12" s="7">
+        <v>3</v>
+      </c>
+      <c r="D12" s="7">
+        <v>4</v>
+      </c>
+      <c r="E12" s="7">
+        <v>5</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+      <c r="G12" s="7">
+        <v>2</v>
+      </c>
+      <c r="H12" s="7">
+        <v>3</v>
+      </c>
+      <c r="I12" s="7">
+        <v>4</v>
+      </c>
+      <c r="J12" s="7">
+        <v>5</v>
+      </c>
+      <c r="K12" s="7">
+        <v>1</v>
+      </c>
+      <c r="L12" s="7">
+        <v>2</v>
+      </c>
+      <c r="M12" s="7">
+        <v>3</v>
+      </c>
+      <c r="N12" s="7">
+        <v>4</v>
+      </c>
+      <c r="O12" s="7">
+        <v>5</v>
+      </c>
+      <c r="P12" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>2</v>
+      </c>
+      <c r="R12" s="7">
+        <v>3</v>
+      </c>
+      <c r="S12" s="7">
+        <v>4</v>
+      </c>
+      <c r="T12" s="7">
+        <v>5</v>
+      </c>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
       <c r="W12" s="7"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7">
-        <v>30</v>
-      </c>
-      <c r="C13" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="C13" s="7">
+        <v>3</v>
+      </c>
       <c r="D13" s="7">
-        <v>30</v>
-      </c>
-      <c r="E13" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="E13" s="7">
+        <v>5</v>
+      </c>
       <c r="F13" s="7">
-        <v>30</v>
-      </c>
-      <c r="G13" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2</v>
+      </c>
       <c r="H13" s="7">
-        <v>30</v>
-      </c>
-      <c r="I13" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="I13" s="7">
+        <v>4</v>
+      </c>
       <c r="J13" s="7">
-        <v>30</v>
-      </c>
-      <c r="K13" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="K13" s="7">
+        <v>1</v>
+      </c>
       <c r="L13" s="7">
-        <v>30</v>
-      </c>
-      <c r="M13" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="M13" s="7">
+        <v>3</v>
+      </c>
       <c r="N13" s="7">
-        <v>30</v>
-      </c>
-      <c r="O13" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="O13" s="7">
+        <v>5</v>
+      </c>
       <c r="P13" s="7">
-        <v>30</v>
-      </c>
-      <c r="Q13" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>2</v>
+      </c>
       <c r="R13" s="7">
-        <v>30</v>
-      </c>
-      <c r="S13" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="S13" s="7">
+        <v>4</v>
+      </c>
       <c r="T13" s="7">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="U13" s="7"/>
       <c r="V13" s="7"/>
       <c r="W13" s="7">
-        <v>300</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1036,96 +1068,100 @@
       <c r="W14" s="5"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>9</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="7">
-        <v>9</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="7">
-        <v>9</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="7">
-        <v>9</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" s="7">
-        <v>9</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K15" s="7">
-        <v>9</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="M15" s="7">
-        <v>9</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O15" s="7">
-        <v>9</v>
-      </c>
-      <c r="P15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q15" s="7">
-        <v>9</v>
-      </c>
-      <c r="R15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="S15" s="7">
-        <v>9</v>
-      </c>
-      <c r="T15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7">
-        <v>90</v>
-      </c>
+      <c r="A15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W15" s="7"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="5"/>
-      <c r="W16" s="5"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7">
+        <v>30</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7">
+        <v>30</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7">
+        <v>30</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7">
+        <v>30</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7">
+        <v>30</v>
+      </c>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7">
+        <v>30</v>
+      </c>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7">
+        <v>30</v>
+      </c>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7">
+        <v>30</v>
+      </c>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7">
+        <v>30</v>
+      </c>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7">
+        <v>30</v>
+      </c>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7">
+        <v>300</v>
+      </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
@@ -1154,117 +1190,95 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G18" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I18" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K18" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M18" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O18" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q18" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R18" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S18" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="U18" s="7">
-        <v>5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="U18" s="7"/>
       <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
+      <c r="W18" s="7">
+        <v>90</v>
+      </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7">
-        <v>15</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7">
-        <v>15</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7">
-        <v>15</v>
-      </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7">
-        <v>15</v>
-      </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7">
-        <v>15</v>
-      </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7">
-        <v>15</v>
-      </c>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7">
-        <v>15</v>
-      </c>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7">
-        <v>15</v>
-      </c>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7">
-        <v>15</v>
-      </c>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7">
-        <v>15</v>
-      </c>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7">
-        <v>150</v>
-      </c>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
@@ -1292,54 +1306,118 @@
       <c r="W20" s="5"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
+      <c r="A21" s="7">
+        <v>5</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="7">
+        <v>5</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="7">
+        <v>5</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="7">
+        <v>5</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="7">
+        <v>5</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21" s="7">
+        <v>5</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" s="7">
+        <v>5</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" s="7">
+        <v>5</v>
+      </c>
+      <c r="P21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>5</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="S21" s="7">
+        <v>5</v>
+      </c>
+      <c r="T21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="U21" s="7">
+        <v>5</v>
+      </c>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
-      <c r="V22" s="5"/>
-      <c r="W22" s="5"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7">
+        <v>15</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7">
+        <v>15</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7">
+        <v>15</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7">
+        <v>15</v>
+      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7">
+        <v>15</v>
+      </c>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7">
+        <v>15</v>
+      </c>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7">
+        <v>15</v>
+      </c>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7">
+        <v>15</v>
+      </c>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7">
+        <v>15</v>
+      </c>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7">
+        <v>150</v>
+      </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
@@ -1416,6 +1494,81 @@
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
     </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="M2:N2"/>

</xml_diff>

<commit_message>
one strike in last frame
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="6">
   <si>
     <t>X</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:W28"/>
+  <dimension ref="A2:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,99 +1068,135 @@
       <c r="W14" s="5"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="R15" s="7"/>
+      <c r="A15" s="7">
+        <v>1</v>
+      </c>
+      <c r="B15" s="7">
+        <v>2</v>
+      </c>
+      <c r="C15" s="7">
+        <v>3</v>
+      </c>
+      <c r="D15" s="7">
+        <v>4</v>
+      </c>
+      <c r="E15" s="7">
+        <v>5</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
+      <c r="G15" s="7">
+        <v>2</v>
+      </c>
+      <c r="H15" s="7">
+        <v>3</v>
+      </c>
+      <c r="I15" s="7">
+        <v>4</v>
+      </c>
+      <c r="J15" s="7">
+        <v>5</v>
+      </c>
+      <c r="K15" s="7">
+        <v>1</v>
+      </c>
+      <c r="L15" s="7">
+        <v>2</v>
+      </c>
+      <c r="M15" s="7">
+        <v>3</v>
+      </c>
+      <c r="N15" s="7">
+        <v>4</v>
+      </c>
+      <c r="O15" s="7">
+        <v>5</v>
+      </c>
+      <c r="P15" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>2</v>
+      </c>
+      <c r="R15" s="7">
+        <v>3</v>
+      </c>
       <c r="S15" s="7" t="s">
         <v>0</v>
       </c>
       <c r="T15" s="7"/>
-      <c r="U15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="V15" s="7" t="s">
-        <v>0</v>
+      <c r="U15" s="7">
+        <v>5</v>
+      </c>
+      <c r="V15" s="7">
+        <v>3</v>
       </c>
       <c r="W15" s="7"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="7">
+        <v>1</v>
+      </c>
       <c r="B16" s="7">
-        <v>30</v>
-      </c>
-      <c r="C16" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3</v>
+      </c>
       <c r="D16" s="7">
-        <v>30</v>
-      </c>
-      <c r="E16" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="E16" s="7">
+        <v>5</v>
+      </c>
       <c r="F16" s="7">
-        <v>30</v>
-      </c>
-      <c r="G16" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="G16" s="7">
+        <v>2</v>
+      </c>
       <c r="H16" s="7">
-        <v>30</v>
-      </c>
-      <c r="I16" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="I16" s="7">
+        <v>4</v>
+      </c>
       <c r="J16" s="7">
-        <v>30</v>
-      </c>
-      <c r="K16" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="K16" s="7">
+        <v>1</v>
+      </c>
       <c r="L16" s="7">
-        <v>30</v>
-      </c>
-      <c r="M16" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="M16" s="7">
+        <v>3</v>
+      </c>
       <c r="N16" s="7">
-        <v>30</v>
-      </c>
-      <c r="O16" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="O16" s="7">
+        <v>5</v>
+      </c>
       <c r="P16" s="7">
-        <v>30</v>
-      </c>
-      <c r="Q16" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>2</v>
+      </c>
       <c r="R16" s="7">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="S16" s="7"/>
       <c r="T16" s="7">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="U16" s="7"/>
       <c r="V16" s="7"/>
       <c r="W16" s="7">
-        <v>300</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -1189,234 +1225,216 @@
       <c r="W17" s="5"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W19" s="7"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7">
+        <v>30</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7">
+        <v>30</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7">
+        <v>30</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7">
+        <v>30</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7">
+        <v>30</v>
+      </c>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7">
+        <v>30</v>
+      </c>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7">
+        <v>30</v>
+      </c>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7">
+        <v>30</v>
+      </c>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7">
+        <v>30</v>
+      </c>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7">
+        <v>30</v>
+      </c>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <v>9</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="7">
+      <c r="B22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="7">
         <v>9</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="7">
+      <c r="D22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="7">
         <v>9</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="7">
+      <c r="F22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="7">
         <v>9</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="7">
+      <c r="H22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="7">
         <v>9</v>
       </c>
-      <c r="J18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K18" s="7">
+      <c r="J22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="7">
         <v>9</v>
       </c>
-      <c r="L18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="M18" s="7">
+      <c r="L22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M22" s="7">
         <v>9</v>
       </c>
-      <c r="N18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O18" s="7">
+      <c r="N22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O22" s="7">
         <v>9</v>
       </c>
-      <c r="P18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q18" s="7">
+      <c r="P22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="7">
         <v>9</v>
       </c>
-      <c r="R18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="S18" s="7">
+      <c r="R22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="S22" s="7">
         <v>9</v>
       </c>
-      <c r="T18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
-      <c r="V20" s="5"/>
-      <c r="W20" s="5"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
-        <v>5</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="7">
-        <v>5</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="7">
-        <v>5</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="7">
-        <v>5</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I21" s="7">
-        <v>5</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K21" s="7">
-        <v>5</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M21" s="7">
-        <v>5</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="O21" s="7">
-        <v>5</v>
-      </c>
-      <c r="P21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q21" s="7">
-        <v>5</v>
-      </c>
-      <c r="R21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="S21" s="7">
-        <v>5</v>
-      </c>
-      <c r="T21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="U21" s="7">
-        <v>5</v>
-      </c>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7">
-        <v>15</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7">
-        <v>15</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7">
-        <v>15</v>
-      </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7">
-        <v>15</v>
-      </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7">
-        <v>15</v>
-      </c>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7">
-        <v>15</v>
-      </c>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7">
-        <v>15</v>
-      </c>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7">
-        <v>15</v>
-      </c>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7">
-        <v>15</v>
-      </c>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7">
-        <v>15</v>
+      <c r="T22" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="U22" s="7"/>
       <c r="V22" s="7"/>
       <c r="W22" s="7">
-        <v>150</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -1470,54 +1488,118 @@
       <c r="W24" s="5"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
+      <c r="A25" s="7">
+        <v>5</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="7">
+        <v>5</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="7">
+        <v>5</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="7">
+        <v>5</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="7">
+        <v>5</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" s="7">
+        <v>5</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M25" s="7">
+        <v>5</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O25" s="7">
+        <v>5</v>
+      </c>
+      <c r="P25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>5</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="S25" s="7">
+        <v>5</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="U25" s="7">
+        <v>5</v>
+      </c>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7">
+        <v>15</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7">
+        <v>15</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7">
+        <v>15</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7">
+        <v>15</v>
+      </c>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7">
+        <v>15</v>
+      </c>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7">
+        <v>15</v>
+      </c>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7">
+        <v>15</v>
+      </c>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7">
+        <v>15</v>
+      </c>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7">
+        <v>15</v>
+      </c>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7">
+        <v>150</v>
+      </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
@@ -1569,6 +1651,106 @@
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
     </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="M2:N2"/>

</xml_diff>